<commit_message>
Change in the Templates folder for the xlsx file name change
</commit_message>
<xml_diff>
--- a/templates/export/events.xlsx
+++ b/templates/export/events.xlsx
@@ -77,7 +77,7 @@
     <t xml:space="preserve">Report type:</t>
   </si>
   <si>
-    <t xml:space="preserve">Events</t>
+    <t xml:space="preserve">Alerts</t>
   </si>
   <si>
     <t xml:space="preserve">Device:</t>
@@ -307,7 +307,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="3" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="6" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -315,7 +315,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="3" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="6" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -434,9 +434,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>3685320</xdr:colOff>
+      <xdr:colOff>3684960</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>140040</xdr:rowOff>
+      <xdr:rowOff>139680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -446,7 +446,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="12556440" cy="9524160"/>
+          <a:ext cx="14875920" cy="9523440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -479,9 +479,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>3685320</xdr:colOff>
+      <xdr:colOff>3684960</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>140040</xdr:rowOff>
+      <xdr:rowOff>139680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -491,7 +491,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="12556440" cy="9524160"/>
+          <a:ext cx="14875920" cy="9523440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -524,9 +524,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>3685320</xdr:colOff>
+      <xdr:colOff>3684960</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>140040</xdr:rowOff>
+      <xdr:rowOff>139680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -536,7 +536,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="12556440" cy="9524160"/>
+          <a:ext cx="14875920" cy="9523440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -569,9 +569,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1132920</xdr:colOff>
+      <xdr:colOff>1132560</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>140040</xdr:rowOff>
+      <xdr:rowOff>139680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -581,7 +581,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10004040" cy="9524160"/>
+          <a:ext cx="12323520" cy="9523440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -589,7 +589,7 @@
         <a:solidFill>
           <a:srgbClr val="ffffff"/>
         </a:solidFill>
-        <a:ln w="9525">
+        <a:ln w="9360">
           <a:solidFill>
             <a:srgbClr val="000000"/>
           </a:solidFill>
@@ -614,9 +614,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1132920</xdr:colOff>
+      <xdr:colOff>1132560</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>140040</xdr:rowOff>
+      <xdr:rowOff>139680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -626,7 +626,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10004040" cy="9524160"/>
+          <a:ext cx="12323520" cy="9523440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -634,7 +634,7 @@
         <a:solidFill>
           <a:srgbClr val="ffffff"/>
         </a:solidFill>
-        <a:ln w="9525">
+        <a:ln w="9360">
           <a:solidFill>
             <a:srgbClr val="000000"/>
           </a:solidFill>
@@ -659,9 +659,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1132920</xdr:colOff>
+      <xdr:colOff>1132560</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>140040</xdr:rowOff>
+      <xdr:rowOff>139680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -671,7 +671,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10004040" cy="9524160"/>
+          <a:ext cx="12323520" cy="9523440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -679,7 +679,7 @@
         <a:solidFill>
           <a:srgbClr val="ffffff"/>
         </a:solidFill>
-        <a:ln w="9525">
+        <a:ln w="9360">
           <a:solidFill>
             <a:srgbClr val="000000"/>
           </a:solidFill>
@@ -699,14 +699,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -831,8 +831,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.747916666666667" bottom="0.747916666666667" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.747916666666667" bottom="0.747916666666667" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>